<commit_message>
final commit to gojek branch
</commit_message>
<xml_diff>
--- a/src/test/resources/com/gojek/xls/Flight Suite.xlsx
+++ b/src/test/resources/com/gojek/xls/Flight Suite.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>TCID</t>
   </si>
@@ -50,9 +50,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
     <t>flight_return_date</t>
   </si>
   <si>
@@ -84,16 +81,12 @@
   </si>
   <si>
     <t>April-30-2017</t>
-  </si>
-  <si>
-    <t>SKIP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -511,15 +504,15 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.58203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="1" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -556,9 +549,7 @@
       <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="D3" s="4"/>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -616,34 +607,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="5" max="7" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="7.58203125" collapsed="true"/>
+    <col min="1" max="2" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="7.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>17</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>2</v>
@@ -657,16 +648,16 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -676,23 +667,21 @@
       <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="E3" s="5">
         <v>2</v>
@@ -702,9 +691,7 @@
       <c r="H3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>23</v>
-      </c>
+      <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
   </sheetData>

</xml_diff>